<commit_message>
EDA using my standard interpolation function
</commit_message>
<xml_diff>
--- a/CH-097 Linear Interpolation.xlsx
+++ b/CH-097 Linear Interpolation.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1705CEB-73C6-447F-A156-32A01454ACFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5162C125-E8F4-45C3-9948-D65D1940166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$5</definedName>
+    <definedName name="fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat,      _xlfn.LET(          _xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.xdat,,-1),          _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.xdat,,1),          _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.ydat,,-1),          _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.ydat,,1),          IF(_xlpm.xmin=_xlpm.xmax,_xlpm.ymin,                      (_xlpm.ymin*(_xlpm.xmax-_xlpm.x)+_xlpm.ymax*(_xlpm.x-_xlpm.xmin))/(_xlpm.xmax-_xlpm.xmin))      ) )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t>Question</t>
   </si>
@@ -57,6 +82,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>My standard function does not extrapolate.</t>
   </si>
 </sst>
 </file>
@@ -317,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -376,6 +404,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -907,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N9:N10"/>
     </sheetView>
   </sheetViews>
@@ -1327,4 +1358,651 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87ACFFC0-BD62-4376-81FA-4B47E0475CF9}">
+  <dimension ref="A1:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="5" width="8.8984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.3984375" customWidth="1"/>
+    <col min="8" max="9" width="8.8984375" style="5" customWidth="1"/>
+    <col min="10" max="11" width="8.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="H1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="H2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>2011</v>
+      </c>
+      <c r="C3" s="15">
+        <v>10</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2282751</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1831961</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="H3" s="16">
+        <v>2010</v>
+      </c>
+      <c r="I3" s="15">
+        <v>9</v>
+      </c>
+      <c r="J3" s="15">
+        <v>2234193</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1799818</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="15">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15">
+        <v>2525540</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1992674</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="H4" s="16">
+        <v>2011</v>
+      </c>
+      <c r="I4" s="15">
+        <v>10</v>
+      </c>
+      <c r="J4" s="15">
+        <v>2282751</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1831961</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="15">
+        <v>25</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2810815</v>
+      </c>
+      <c r="E5" s="15">
+        <v>2195595</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="H5" s="16">
+        <v>2012</v>
+      </c>
+      <c r="I5" s="15">
+        <v>11</v>
+      </c>
+      <c r="J5" s="15">
+        <v>2331309</v>
+      </c>
+      <c r="K5" s="13">
+        <v>1864104</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="9"/>
+      <c r="H6" s="16">
+        <v>2013</v>
+      </c>
+      <c r="I6" s="15">
+        <v>12</v>
+      </c>
+      <c r="J6" s="15">
+        <v>2379867</v>
+      </c>
+      <c r="K6" s="13">
+        <v>1896246</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="9"/>
+      <c r="H7" s="16">
+        <v>2014</v>
+      </c>
+      <c r="I7" s="15">
+        <v>13</v>
+      </c>
+      <c r="J7" s="15">
+        <v>2428424</v>
+      </c>
+      <c r="K7" s="13">
+        <v>1928389</v>
+      </c>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="b" cm="1">
+        <f t="array" ref="B8:E10">ISNUMBER(B3:E5)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8"/>
+      <c r="H8" s="16">
+        <v>2015</v>
+      </c>
+      <c r="I8" s="15">
+        <v>14</v>
+      </c>
+      <c r="J8" s="15">
+        <v>2476982</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1960531</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9"/>
+      <c r="H9" s="16">
+        <v>2016</v>
+      </c>
+      <c r="I9" s="15">
+        <v>15</v>
+      </c>
+      <c r="J9" s="15">
+        <v>2525540</v>
+      </c>
+      <c r="K9" s="13">
+        <v>1992674</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10"/>
+      <c r="H10" s="16">
+        <v>2017</v>
+      </c>
+      <c r="I10" s="15">
+        <v>17</v>
+      </c>
+      <c r="J10" s="15">
+        <v>2582595</v>
+      </c>
+      <c r="K10" s="13">
+        <v>2033258</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="9"/>
+      <c r="G11"/>
+      <c r="H11" s="16">
+        <v>2018</v>
+      </c>
+      <c r="I11" s="15">
+        <v>19</v>
+      </c>
+      <c r="J11" s="15">
+        <v>2639650</v>
+      </c>
+      <c r="K11" s="13">
+        <v>2073842</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="9"/>
+      <c r="G12"/>
+      <c r="H12" s="16">
+        <v>2019</v>
+      </c>
+      <c r="I12" s="15">
+        <v>21</v>
+      </c>
+      <c r="J12" s="15">
+        <v>2696705</v>
+      </c>
+      <c r="K12" s="13">
+        <v>2114427</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="9"/>
+      <c r="H13" s="16">
+        <v>2020</v>
+      </c>
+      <c r="I13" s="15">
+        <v>23</v>
+      </c>
+      <c r="J13" s="15">
+        <v>2753760</v>
+      </c>
+      <c r="K13" s="13">
+        <v>2155011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F14" s="9"/>
+      <c r="H14" s="16">
+        <v>2021</v>
+      </c>
+      <c r="I14" s="15">
+        <v>25</v>
+      </c>
+      <c r="J14" s="15">
+        <v>2810815</v>
+      </c>
+      <c r="K14" s="13">
+        <v>2195595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="F15" s="9"/>
+      <c r="H15" s="17">
+        <v>2022</v>
+      </c>
+      <c r="I15" s="18">
+        <v>27</v>
+      </c>
+      <c r="J15" s="18">
+        <v>2867870</v>
+      </c>
+      <c r="K15" s="14">
+        <v>2236179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="C17" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="C19" s="4" cm="1">
+        <f t="array" ref="C19:C31">H3:H15</f>
+        <v>2010</v>
+      </c>
+      <c r="D19" s="4" t="e" cm="1">
+        <f t="array" ref="D19">fInterp($C19,$B$3:$B$5,C$3:C$5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E19" s="4" t="e" cm="1">
+        <f t="array" ref="E19">fInterp($C19,$B$3:$B$5,D$3:D$5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F19" s="4" t="e" cm="1">
+        <f t="array" ref="F19">fInterp($C19,$B$3:$B$5,E$3:E$5)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="C20" s="4">
+        <v>2011</v>
+      </c>
+      <c r="D20" s="4" cm="1">
+        <f t="array" ref="D20">fInterp($C20,$B$3:$B$5,C$3:C$5)</f>
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" cm="1">
+        <f t="array" ref="E20">fInterp($C20,$B$3:$B$5,D$3:D$5)</f>
+        <v>2282751</v>
+      </c>
+      <c r="F20" s="4" cm="1">
+        <f t="array" ref="F20">fInterp($C20,$B$3:$B$5,E$3:E$5)</f>
+        <v>1831961</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="C21" s="4">
+        <v>2012</v>
+      </c>
+      <c r="D21" s="4" cm="1">
+        <f t="array" ref="D21">fInterp($C21,$B$3:$B$5,C$3:C$5)</f>
+        <v>11</v>
+      </c>
+      <c r="E21" s="4" cm="1">
+        <f t="array" ref="E21">fInterp($C21,$B$3:$B$5,D$3:D$5)</f>
+        <v>2331308.7999999998</v>
+      </c>
+      <c r="F21" s="4" cm="1">
+        <f t="array" ref="F21">fInterp($C21,$B$3:$B$5,E$3:E$5)</f>
+        <v>1864103.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="C22" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D22" s="4" cm="1">
+        <f t="array" ref="D22">fInterp($C22,$B$3:$B$5,C$3:C$5)</f>
+        <v>12</v>
+      </c>
+      <c r="E22" s="4" cm="1">
+        <f t="array" ref="E22">fInterp($C22,$B$3:$B$5,D$3:D$5)</f>
+        <v>2379866.6</v>
+      </c>
+      <c r="F22" s="4" cm="1">
+        <f t="array" ref="F22">fInterp($C22,$B$3:$B$5,E$3:E$5)</f>
+        <v>1896246.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="C23" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D23" s="4" cm="1">
+        <f t="array" ref="D23">fInterp($C23,$B$3:$B$5,C$3:C$5)</f>
+        <v>13</v>
+      </c>
+      <c r="E23" s="4" cm="1">
+        <f t="array" ref="E23">fInterp($C23,$B$3:$B$5,D$3:D$5)</f>
+        <v>2428424.4</v>
+      </c>
+      <c r="F23" s="4" cm="1">
+        <f t="array" ref="F23">fInterp($C23,$B$3:$B$5,E$3:E$5)</f>
+        <v>1928388.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
+        <v>2015</v>
+      </c>
+      <c r="D24" s="4" cm="1">
+        <f t="array" ref="D24">fInterp($C24,$B$3:$B$5,C$3:C$5)</f>
+        <v>14</v>
+      </c>
+      <c r="E24" s="4" cm="1">
+        <f t="array" ref="E24">fInterp($C24,$B$3:$B$5,D$3:D$5)</f>
+        <v>2476982.2000000002</v>
+      </c>
+      <c r="F24" s="4" cm="1">
+        <f t="array" ref="F24">fInterp($C24,$B$3:$B$5,E$3:E$5)</f>
+        <v>1960531.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>2016</v>
+      </c>
+      <c r="D25" s="4" cm="1">
+        <f t="array" ref="D25">fInterp($C25,$B$3:$B$5,C$3:C$5)</f>
+        <v>15</v>
+      </c>
+      <c r="E25" s="4" cm="1">
+        <f t="array" ref="E25">fInterp($C25,$B$3:$B$5,D$3:D$5)</f>
+        <v>2525540</v>
+      </c>
+      <c r="F25" s="4" cm="1">
+        <f t="array" ref="F25">fInterp($C25,$B$3:$B$5,E$3:E$5)</f>
+        <v>1992674</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="4">
+        <v>2017</v>
+      </c>
+      <c r="D26" s="4" cm="1">
+        <f t="array" ref="D26">fInterp($C26,$B$3:$B$5,C$3:C$5)</f>
+        <v>17</v>
+      </c>
+      <c r="E26" s="4" cm="1">
+        <f t="array" ref="E26">fInterp($C26,$B$3:$B$5,D$3:D$5)</f>
+        <v>2582595</v>
+      </c>
+      <c r="F26" s="4" cm="1">
+        <f t="array" ref="F26">fInterp($C26,$B$3:$B$5,E$3:E$5)</f>
+        <v>2033258.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D27" s="4" cm="1">
+        <f t="array" ref="D27">fInterp($C27,$B$3:$B$5,C$3:C$5)</f>
+        <v>19</v>
+      </c>
+      <c r="E27" s="4" cm="1">
+        <f t="array" ref="E27">fInterp($C27,$B$3:$B$5,D$3:D$5)</f>
+        <v>2639650</v>
+      </c>
+      <c r="F27" s="4" cm="1">
+        <f t="array" ref="F27">fInterp($C27,$B$3:$B$5,E$3:E$5)</f>
+        <v>2073842.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D28" s="4" cm="1">
+        <f t="array" ref="D28">fInterp($C28,$B$3:$B$5,C$3:C$5)</f>
+        <v>21</v>
+      </c>
+      <c r="E28" s="4" cm="1">
+        <f t="array" ref="E28">fInterp($C28,$B$3:$B$5,D$3:D$5)</f>
+        <v>2696705</v>
+      </c>
+      <c r="F28" s="4" cm="1">
+        <f t="array" ref="F28">fInterp($C28,$B$3:$B$5,E$3:E$5)</f>
+        <v>2114426.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="4">
+        <v>2020</v>
+      </c>
+      <c r="D29" s="4" cm="1">
+        <f t="array" ref="D29">fInterp($C29,$B$3:$B$5,C$3:C$5)</f>
+        <v>23</v>
+      </c>
+      <c r="E29" s="4" cm="1">
+        <f t="array" ref="E29">fInterp($C29,$B$3:$B$5,D$3:D$5)</f>
+        <v>2753760</v>
+      </c>
+      <c r="F29" s="4" cm="1">
+        <f t="array" ref="F29">fInterp($C29,$B$3:$B$5,E$3:E$5)</f>
+        <v>2155010.7999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="4">
+        <v>2021</v>
+      </c>
+      <c r="D30" s="4" cm="1">
+        <f t="array" ref="D30">fInterp($C30,$B$3:$B$5,C$3:C$5)</f>
+        <v>25</v>
+      </c>
+      <c r="E30" s="4" cm="1">
+        <f t="array" ref="E30">fInterp($C30,$B$3:$B$5,D$3:D$5)</f>
+        <v>2810815</v>
+      </c>
+      <c r="F30" s="4" cm="1">
+        <f t="array" ref="F30">fInterp($C30,$B$3:$B$5,E$3:E$5)</f>
+        <v>2195595</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="4">
+        <v>2022</v>
+      </c>
+      <c r="D31" s="4" t="e" cm="1">
+        <f t="array" ref="D31">fInterp($C31,$B$3:$B$5,C$3:C$5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E31" s="4" t="e" cm="1">
+        <f t="array" ref="E31">fInterp($C31,$B$3:$B$5,D$3:D$5)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F31" s="4" t="e" cm="1">
+        <f t="array" ref="F31">fInterp($C31,$B$3:$B$5,E$3:E$5)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Trying an ALT using trend
</commit_message>
<xml_diff>
--- a/CH-097 Linear Interpolation.xlsx
+++ b/CH-097 Linear Interpolation.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5162C125-E8F4-45C3-9948-D65D1940166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB87FA24-07FE-4130-8C79-A3C8109CBE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$5</definedName>
     <definedName name="fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat,      _xlfn.LET(          _xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.xdat,,-1),          _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.xdat,,1),          _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.ydat,,-1),          _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.ydat,,1),          IF(_xlpm.xmin=_xlpm.xmax,_xlpm.ymin,                      (_xlpm.ymin*(_xlpm.xmax-_xlpm.x)+_xlpm.ymax*(_xlpm.x-_xlpm.xmin))/(_xlpm.xmax-_xlpm.xmin))      ) )</definedName>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -86,12 +88,15 @@
   <si>
     <t>My standard function does not extrapolate.</t>
   </si>
+  <si>
+    <t>https://www.linkedin.com/feed/update/urn:li:activity:7229230243260022785/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +132,14 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -342,10 +355,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,6 +407,9 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -405,11 +422,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -641,6 +659,154 @@
         <a:xfrm rot="5400000">
           <a:off x="3095625" y="390525"/>
           <a:ext cx="701675" cy="1012825"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1098550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19849</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>125767</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Right 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FDA41F1-F3FC-434E-B51D-1021822F21A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4977130" y="1329523"/>
+          <a:ext cx="323379" cy="655524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>92075</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Arrow: Bent 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D5AE31C-67C7-4125-9695-04585D82CE40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3120390" y="381000"/>
+          <a:ext cx="691515" cy="1009015"/>
         </a:xfrm>
         <a:prstGeom prst="bentArrow">
           <a:avLst/>
@@ -934,12 +1100,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="902" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{515F7D46-1555-46AB-933C-E6E4B5A055AF}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N9:N10"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -953,18 +1146,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="H1" s="21" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="24" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1354,9 +1550,12 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M1" r:id="rId1" xr:uid="{40D954C3-A74C-4DB7-9BA1-0DC7887F7183}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1364,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87ACFFC0-BD62-4376-81FA-4B47E0475CF9}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -1379,18 +1578,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="H1" s="21" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="H1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1761,7 +1960,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="19" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="9"/>
@@ -2005,4 +2204,613 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7DDB07-353D-4E20-83DB-DA29E5CD4726}">
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="5" width="8.8984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.3984375" customWidth="1"/>
+    <col min="8" max="9" width="8.8984375" style="5" customWidth="1"/>
+    <col min="10" max="11" width="8.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="H1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="M1" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="H2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>2011</v>
+      </c>
+      <c r="C3" s="15">
+        <v>10</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2282751</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1831961</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="H3" s="16">
+        <v>2010</v>
+      </c>
+      <c r="I3" s="15">
+        <v>9</v>
+      </c>
+      <c r="J3" s="15">
+        <v>2234193</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1799818</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="15">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15">
+        <v>2525540</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1992674</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="H4" s="16">
+        <v>2011</v>
+      </c>
+      <c r="I4" s="15">
+        <v>10</v>
+      </c>
+      <c r="J4" s="15">
+        <v>2282751</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1831961</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="15">
+        <v>25</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2810815</v>
+      </c>
+      <c r="E5" s="15">
+        <v>2195595</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="H5" s="16">
+        <v>2012</v>
+      </c>
+      <c r="I5" s="15">
+        <v>11</v>
+      </c>
+      <c r="J5" s="15">
+        <v>2331309</v>
+      </c>
+      <c r="K5" s="13">
+        <v>1864104</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="9"/>
+      <c r="H6" s="16">
+        <v>2013</v>
+      </c>
+      <c r="I6" s="15">
+        <v>12</v>
+      </c>
+      <c r="J6" s="15">
+        <v>2379867</v>
+      </c>
+      <c r="K6" s="13">
+        <v>1896246</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="9"/>
+      <c r="H7" s="16">
+        <v>2014</v>
+      </c>
+      <c r="I7" s="15">
+        <v>13</v>
+      </c>
+      <c r="J7" s="15">
+        <v>2428424</v>
+      </c>
+      <c r="K7" s="13">
+        <v>1928389</v>
+      </c>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="9"/>
+      <c r="G8"/>
+      <c r="H8" s="16">
+        <v>2015</v>
+      </c>
+      <c r="I8" s="15">
+        <v>14</v>
+      </c>
+      <c r="J8" s="15">
+        <v>2476982</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1960531</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="9"/>
+      <c r="G9"/>
+      <c r="H9" s="16">
+        <v>2016</v>
+      </c>
+      <c r="I9" s="15">
+        <v>15</v>
+      </c>
+      <c r="J9" s="15">
+        <v>2525540</v>
+      </c>
+      <c r="K9" s="13">
+        <v>1992674</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="9"/>
+      <c r="G10"/>
+      <c r="H10" s="16">
+        <v>2017</v>
+      </c>
+      <c r="I10" s="15">
+        <v>17</v>
+      </c>
+      <c r="J10" s="15">
+        <v>2582595</v>
+      </c>
+      <c r="K10" s="13">
+        <v>2033258</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="9"/>
+      <c r="G11"/>
+      <c r="H11" s="16">
+        <v>2018</v>
+      </c>
+      <c r="I11" s="15">
+        <v>19</v>
+      </c>
+      <c r="J11" s="15">
+        <v>2639650</v>
+      </c>
+      <c r="K11" s="13">
+        <v>2073842</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="9"/>
+      <c r="G12"/>
+      <c r="H12" s="16">
+        <v>2019</v>
+      </c>
+      <c r="I12" s="15">
+        <v>21</v>
+      </c>
+      <c r="J12" s="15">
+        <v>2696705</v>
+      </c>
+      <c r="K12" s="13">
+        <v>2114427</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="9"/>
+      <c r="H13" s="16">
+        <v>2020</v>
+      </c>
+      <c r="I13" s="15">
+        <v>23</v>
+      </c>
+      <c r="J13" s="15">
+        <v>2753760</v>
+      </c>
+      <c r="K13" s="13">
+        <v>2155011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F14" s="9"/>
+      <c r="H14" s="16">
+        <v>2021</v>
+      </c>
+      <c r="I14" s="15">
+        <v>25</v>
+      </c>
+      <c r="J14" s="15">
+        <v>2810815</v>
+      </c>
+      <c r="K14" s="13">
+        <v>2195595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4" cm="1">
+        <f t="array" ref="B15:E27">_xlfn.LET(
+    _xlpm.y, B3:B5,
+    _xlpm.s, _xlfn.SEQUENCE(13, , 2010),
+    _xlfn.REDUCE(
+        _xlpm.s,
+        C3:E3,
+        _xlfn.LAMBDA(_xlpm.a,_xlpm.c,
+            _xlfn.HSTACK(
+                _xlpm.a,
+                _xlfn.MAP(
+                    _xlpm.s,
+                    _xlfn.LAMBDA(_xlpm.w,
+                        _xlfn.LET(
+                            _xlpm.n, MATCH(MEDIAN(_xlpm.w, _xlpm.y), _xlpm.y) + {0;1},
+                            TREND(INDEX(E5:_xlpm.c, _xlpm.n, 1), INDEX(_xlpm.y, _xlpm.n), _xlpm.w)
+                        )
+                    )
+                )
+            )
+        )
+    )
+)</f>
+        <v>2010</v>
+      </c>
+      <c r="C15" s="4">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2234193.1999999881</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1799818.400000006</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="H15" s="17">
+        <v>2022</v>
+      </c>
+      <c r="I15" s="18">
+        <v>27</v>
+      </c>
+      <c r="J15" s="18">
+        <v>2867870</v>
+      </c>
+      <c r="K15" s="14">
+        <v>2236179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4">
+        <v>2011</v>
+      </c>
+      <c r="C16" s="4">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4">
+        <v>2282751</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1831961</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4">
+        <v>2012</v>
+      </c>
+      <c r="C17" s="4">
+        <v>11</v>
+      </c>
+      <c r="D17" s="4">
+        <v>2331308.799999997</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1864103.6000000015</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4">
+        <v>2013</v>
+      </c>
+      <c r="C18" s="4">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4">
+        <v>2379866.599999994</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1896246.200000003</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C19" s="4">
+        <v>13</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2428424.3999999911</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1928388.8000000045</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="4">
+        <v>2015</v>
+      </c>
+      <c r="C20" s="4">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2476982.1999999881</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1960531.400000006</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C21" s="4">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2525540</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1992674</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C22" s="4">
+        <v>17</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2582595</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2033258.200000003</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="4">
+        <v>2018</v>
+      </c>
+      <c r="C23" s="4">
+        <v>19</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2639650</v>
+      </c>
+      <c r="E23" s="4">
+        <v>2073842.400000006</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C24" s="4">
+        <v>21</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2696705</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2114426.6000000089</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C25" s="4">
+        <v>23</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2753760</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2155010.8000000119</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C26" s="4">
+        <v>25</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2810815</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2195595</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>2022</v>
+      </c>
+      <c r="C27" s="4">
+        <v>27</v>
+      </c>
+      <c r="D27" s="4">
+        <v>2867870</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2236179.200000003</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="M1" r:id="rId1" xr:uid="{1FDA400C-46A9-4247-9D0A-F419D2A285D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Time for bed. Intermediate results
</commit_message>
<xml_diff>
--- a/CH-097 Linear Interpolation.xlsx
+++ b/CH-097 Linear Interpolation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A427129-EDCF-4821-89BF-7088060E7B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEB586E-282D-48F8-A05A-D3E588AFB6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
   <si>
     <t>Question</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7229230243260022785/</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -143,7 +152,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -361,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -427,6 +442,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2213,10 +2234,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7DDB07-353D-4E20-83DB-DA29E5CD4726}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L5:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2229,7 +2250,7 @@
     <col min="10" max="11" width="8.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
@@ -2246,7 +2267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
@@ -2273,7 +2294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16">
         <v>2011</v>
       </c>
@@ -2305,7 +2326,7 @@
       <c r="O3" s="11"/>
       <c r="P3" s="9"/>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="16">
         <v>2016</v>
       </c>
@@ -2337,7 +2358,7 @@
       <c r="O4" s="11"/>
       <c r="P4" s="9"/>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16">
         <v>2021</v>
       </c>
@@ -2369,7 +2390,7 @@
       <c r="O5" s="11"/>
       <c r="P5" s="9"/>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
@@ -2393,7 +2414,7 @@
       <c r="O6" s="11"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2413,7 +2434,7 @@
       </c>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -2438,7 +2459,7 @@
       <c r="O8"/>
       <c r="P8"/>
     </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -2463,7 +2484,7 @@
       <c r="O9"/>
       <c r="P9"/>
     </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -2488,7 +2509,7 @@
       <c r="O10"/>
       <c r="P10"/>
     </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -2513,7 +2534,7 @@
       <c r="O11"/>
       <c r="P11"/>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -2534,11 +2555,17 @@
       </c>
       <c r="L12"/>
       <c r="M12"/>
-      <c r="N12"/>
-      <c r="O12"/>
-      <c r="P12"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F13" s="9"/>
       <c r="H13" s="16">
         <v>2020</v>
@@ -2552,8 +2579,30 @@
       <c r="K13" s="13">
         <v>2155011</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>2010</v>
+      </c>
+      <c r="O13">
+        <v>2010</v>
+      </c>
+      <c r="P13" cm="1">
+        <f t="array" ref="P13:P15">B3:B5</f>
+        <v>2011</v>
+      </c>
+      <c r="Q13">
+        <f>MEDIAN(N13,_xlfn.ANCHORARRAY( P13))</f>
+        <v>2013.5</v>
+      </c>
+      <c r="R13" cm="1">
+        <f t="array" ref="R13:R14">MATCH(MEDIAN(N13,_xlfn.ANCHORARRAY( P13)),_xlfn.ANCHORARRAY( P13)) + {0;1}</f>
+        <v>1</v>
+      </c>
+      <c r="S13" s="25" cm="1">
+        <f t="array" ref="S13">TREND(INDEX(E3:E5,_xlfn.ANCHORARRAY( R13), 1), INDEX(_xlfn.ANCHORARRAY(P13),_xlfn.ANCHORARRAY( R13)), N13)</f>
+        <v>1799818.400000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F14" s="9"/>
       <c r="H14" s="16">
         <v>2021</v>
@@ -2567,8 +2616,14 @@
       <c r="K14" s="13">
         <v>2195595</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>2016</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4" cm="1">
         <f t="array" ref="B15:E27">_xlfn.LET(
@@ -2617,8 +2672,11 @@
       <c r="K15" s="14">
         <v>2236179</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="4">
         <v>2011</v>
@@ -2626,7 +2684,7 @@
       <c r="C16" s="4">
         <v>10</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="26">
         <v>2282751</v>
       </c>
       <c r="E16" s="4">
@@ -2634,7 +2692,7 @@
       </c>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="4">
         <v>2012</v>
@@ -2642,7 +2700,7 @@
       <c r="C17" s="4">
         <v>11</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="26">
         <v>2331308.799999997</v>
       </c>
       <c r="E17" s="4">
@@ -2650,7 +2708,7 @@
       </c>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="4">
         <v>2013</v>
@@ -2658,15 +2716,27 @@
       <c r="C18" s="4">
         <v>12</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="26">
         <v>2379866.599999994</v>
       </c>
       <c r="E18" s="4">
         <v>1896246.200000003</v>
       </c>
       <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="27" cm="1">
+        <f t="array" ref="G18:G22">TREND(D3:D4,B3:B4,B16:B20)</f>
+        <v>2282751</v>
+      </c>
+      <c r="I18" s="5" cm="1">
+        <f t="array" ref="I18:I19">TREND(C3:C4,B3:B4,B15:B16)</f>
+        <v>9</v>
+      </c>
+      <c r="J18" s="28" cm="1">
+        <f t="array" ref="J18:J19">MATCH(MEDIAN(B15,B3:B5),B3:B5)+{0;1}</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="4">
         <v>2014</v>
@@ -2674,15 +2744,24 @@
       <c r="C19" s="4">
         <v>13</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="26">
         <v>2428424.3999999911</v>
       </c>
       <c r="E19" s="4">
         <v>1928388.8000000045</v>
       </c>
       <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="27">
+        <v>2331308.799999997</v>
+      </c>
+      <c r="I19" s="5">
+        <v>10</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="4">
         <v>2015</v>
@@ -2690,15 +2769,18 @@
       <c r="C20" s="4">
         <v>14</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="26">
         <v>2476982.1999999881</v>
       </c>
       <c r="E20" s="4">
         <v>1960531.400000006</v>
       </c>
       <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="27">
+        <v>2379866.599999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="4">
         <v>2016</v>
@@ -2713,8 +2795,11 @@
         <v>1992674</v>
       </c>
       <c r="F21" s="9"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="27">
+        <v>2428424.3999999911</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="4">
         <v>2017</v>
@@ -2729,8 +2814,11 @@
         <v>2033258.200000003</v>
       </c>
       <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="27">
+        <v>2476982.1999999881</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="4">
         <v>2018</v>
@@ -2746,7 +2834,7 @@
       </c>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>2019</v>
       </c>
@@ -2761,7 +2849,7 @@
       </c>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>2020</v>
       </c>
@@ -2776,7 +2864,7 @@
       </c>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>2021</v>
       </c>
@@ -2791,7 +2879,7 @@
       </c>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>2022</v>
       </c>

</xml_diff>

<commit_message>
I think I now understand the Alt approaches
</commit_message>
<xml_diff>
--- a/CH-097 Linear Interpolation.xlsx
+++ b/CH-097 Linear Interpolation.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEB586E-282D-48F8-A05A-D3E588AFB6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33149A04-D024-4DC7-9DFD-1E5912577597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="4" r:id="rId4"/>
+    <sheet name="Alt3" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$E$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$B$2:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$E$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$E$5</definedName>
     <definedName name="fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat,      _xlfn.LET(          _xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.xdat,,-1),          _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.xdat,,1),          _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.ydat,,-1),          _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x,_xlpm.xdat,_xlpm.ydat,,1),          IF(_xlpm.xmin=_xlpm.xmax,_xlpm.ymin,                      (_xlpm.ymin*(_xlpm.xmax-_xlpm.x)+_xlpm.ymax*(_xlpm.x-_xlpm.xmin))/(_xlpm.xmax-_xlpm.xmin))      ) )</definedName>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="11">
   <si>
     <t>Question</t>
   </si>
@@ -430,6 +432,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -442,12 +450,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1172,18 +1174,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
       <c r="M1" s="20" t="s">
         <v>7</v>
       </c>
@@ -1589,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87ACFFC0-BD62-4376-81FA-4B47E0475CF9}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1604,18 +1606,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -2236,8 +2238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA7DDB07-353D-4E20-83DB-DA29E5CD4726}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L5:L6"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2251,18 +2253,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
       <c r="M1" s="20" t="s">
         <v>7</v>
       </c>
@@ -2597,7 +2599,7 @@
         <f t="array" ref="R13:R14">MATCH(MEDIAN(N13,_xlfn.ANCHORARRAY( P13)),_xlfn.ANCHORARRAY( P13)) + {0;1}</f>
         <v>1</v>
       </c>
-      <c r="S13" s="25" cm="1">
+      <c r="S13" s="21" cm="1">
         <f t="array" ref="S13">TREND(INDEX(E3:E5,_xlfn.ANCHORARRAY( R13), 1), INDEX(_xlfn.ANCHORARRAY(P13),_xlfn.ANCHORARRAY( R13)), N13)</f>
         <v>1799818.400000006</v>
       </c>
@@ -2684,7 +2686,7 @@
       <c r="C16" s="4">
         <v>10</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="22">
         <v>2282751</v>
       </c>
       <c r="E16" s="4">
@@ -2700,7 +2702,7 @@
       <c r="C17" s="4">
         <v>11</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="22">
         <v>2331308.799999997</v>
       </c>
       <c r="E17" s="4">
@@ -2716,14 +2718,14 @@
       <c r="C18" s="4">
         <v>12</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="22">
         <v>2379866.599999994</v>
       </c>
       <c r="E18" s="4">
         <v>1896246.200000003</v>
       </c>
       <c r="F18" s="9"/>
-      <c r="G18" s="27" cm="1">
+      <c r="G18" s="23" cm="1">
         <f t="array" ref="G18:G22">TREND(D3:D4,B3:B4,B16:B20)</f>
         <v>2282751</v>
       </c>
@@ -2731,7 +2733,7 @@
         <f t="array" ref="I18:I19">TREND(C3:C4,B3:B4,B15:B16)</f>
         <v>9</v>
       </c>
-      <c r="J18" s="28" cm="1">
+      <c r="J18" s="24" cm="1">
         <f t="array" ref="J18:J19">MATCH(MEDIAN(B15,B3:B5),B3:B5)+{0;1}</f>
         <v>1</v>
       </c>
@@ -2744,14 +2746,14 @@
       <c r="C19" s="4">
         <v>13</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="22">
         <v>2428424.3999999911</v>
       </c>
       <c r="E19" s="4">
         <v>1928388.8000000045</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="27">
+      <c r="G19" s="23">
         <v>2331308.799999997</v>
       </c>
       <c r="I19" s="5">
@@ -2769,14 +2771,14 @@
       <c r="C20" s="4">
         <v>14</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="22">
         <v>2476982.1999999881</v>
       </c>
       <c r="E20" s="4">
         <v>1960531.400000006</v>
       </c>
       <c r="F20" s="9"/>
-      <c r="G20" s="27">
+      <c r="G20" s="23">
         <v>2379866.599999994</v>
       </c>
     </row>
@@ -2795,7 +2797,7 @@
         <v>1992674</v>
       </c>
       <c r="F21" s="9"/>
-      <c r="G21" s="27">
+      <c r="G21" s="23">
         <v>2428424.3999999911</v>
       </c>
     </row>
@@ -2814,7 +2816,7 @@
         <v>2033258.200000003</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="G22" s="27">
+      <c r="G22" s="23">
         <v>2476982.1999999881</v>
       </c>
     </row>
@@ -2912,7 +2914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17CDBB6-6407-45B9-A6D1-E739D6B53A87}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2927,18 +2929,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="H1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
       <c r="M1" s="20" t="s">
         <v>7</v>
       </c>
@@ -3541,4 +3543,579 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12755AD6-294A-41B9-AB10-5F5BAD419989}">
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="5" width="8.8984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" customWidth="1"/>
+    <col min="7" max="7" width="18.3984375" customWidth="1"/>
+    <col min="8" max="9" width="8.8984375" style="5" customWidth="1"/>
+    <col min="10" max="11" width="8.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="H1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="M1" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="H2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>2011</v>
+      </c>
+      <c r="C3" s="15">
+        <v>10</v>
+      </c>
+      <c r="D3" s="15">
+        <v>2282751</v>
+      </c>
+      <c r="E3" s="15">
+        <v>1831961</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="H3" s="16">
+        <v>2010</v>
+      </c>
+      <c r="I3" s="15">
+        <v>9</v>
+      </c>
+      <c r="J3" s="15">
+        <v>2234193</v>
+      </c>
+      <c r="K3" s="13">
+        <v>1799818</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="15">
+        <v>15</v>
+      </c>
+      <c r="D4" s="15">
+        <v>2525540</v>
+      </c>
+      <c r="E4" s="15">
+        <v>1992674</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="H4" s="16">
+        <v>2011</v>
+      </c>
+      <c r="I4" s="15">
+        <v>10</v>
+      </c>
+      <c r="J4" s="15">
+        <v>2282751</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1831961</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16">
+        <v>2021</v>
+      </c>
+      <c r="C5" s="15">
+        <v>25</v>
+      </c>
+      <c r="D5" s="15">
+        <v>2810815</v>
+      </c>
+      <c r="E5" s="15">
+        <v>2195595</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="H5" s="16">
+        <v>2012</v>
+      </c>
+      <c r="I5" s="15">
+        <v>11</v>
+      </c>
+      <c r="J5" s="15">
+        <v>2331309</v>
+      </c>
+      <c r="K5" s="13">
+        <v>1864104</v>
+      </c>
+      <c r="L5" s="12"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="9"/>
+      <c r="H6" s="16">
+        <v>2013</v>
+      </c>
+      <c r="I6" s="15">
+        <v>12</v>
+      </c>
+      <c r="J6" s="15">
+        <v>2379867</v>
+      </c>
+      <c r="K6" s="13">
+        <v>1896246</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="9"/>
+      <c r="H7" s="16">
+        <v>2014</v>
+      </c>
+      <c r="I7" s="15">
+        <v>13</v>
+      </c>
+      <c r="J7" s="15">
+        <v>2428424</v>
+      </c>
+      <c r="K7" s="13">
+        <v>1928389</v>
+      </c>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="9"/>
+      <c r="G8"/>
+      <c r="H8" s="16">
+        <v>2015</v>
+      </c>
+      <c r="I8" s="15">
+        <v>14</v>
+      </c>
+      <c r="J8" s="15">
+        <v>2476982</v>
+      </c>
+      <c r="K8" s="13">
+        <v>1960531</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="9"/>
+      <c r="G9"/>
+      <c r="H9" s="16">
+        <v>2016</v>
+      </c>
+      <c r="I9" s="15">
+        <v>15</v>
+      </c>
+      <c r="J9" s="15">
+        <v>2525540</v>
+      </c>
+      <c r="K9" s="13">
+        <v>1992674</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="9"/>
+      <c r="G10"/>
+      <c r="H10" s="16">
+        <v>2017</v>
+      </c>
+      <c r="I10" s="15">
+        <v>17</v>
+      </c>
+      <c r="J10" s="15">
+        <v>2582595</v>
+      </c>
+      <c r="K10" s="13">
+        <v>2033258</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="9"/>
+      <c r="G11"/>
+      <c r="H11" s="16">
+        <v>2018</v>
+      </c>
+      <c r="I11" s="15">
+        <v>19</v>
+      </c>
+      <c r="J11" s="15">
+        <v>2639650</v>
+      </c>
+      <c r="K11" s="13">
+        <v>2073842</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="9"/>
+      <c r="G12"/>
+      <c r="H12" s="16">
+        <v>2019</v>
+      </c>
+      <c r="I12" s="15">
+        <v>21</v>
+      </c>
+      <c r="J12" s="15">
+        <v>2696705</v>
+      </c>
+      <c r="K12" s="13">
+        <v>2114427</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>2011</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2009</v>
+      </c>
+      <c r="D13" s="4" cm="1">
+        <f t="array" ref="D13:D26">_xlfn.MAP(C13:C26,_xlfn.LAMBDA(_xlpm.x,MATCH(MEDIAN(_xlpm.x,B3:B5),B3:B5)))</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="4" cm="1">
+        <f t="array" ref="E13:E26">_xlfn.MAP(C13:C26,_xlfn.LAMBDA(_xlpm.x,MATCH(MEDIAN(_xlpm.x,B13:B18),B13:B18)))</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="H13" s="16">
+        <v>2020</v>
+      </c>
+      <c r="I13" s="15">
+        <v>23</v>
+      </c>
+      <c r="J13" s="15">
+        <v>2753760</v>
+      </c>
+      <c r="K13" s="13">
+        <v>2155011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>2013</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2010</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="H14" s="16">
+        <v>2021</v>
+      </c>
+      <c r="I14" s="15">
+        <v>25</v>
+      </c>
+      <c r="J14" s="15">
+        <v>2810815</v>
+      </c>
+      <c r="K14" s="13">
+        <v>2195595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4">
+        <v>2015</v>
+      </c>
+      <c r="C15" s="4">
+        <v>2011</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="H15" s="17">
+        <v>2022</v>
+      </c>
+      <c r="I15" s="18">
+        <v>27</v>
+      </c>
+      <c r="J15" s="18">
+        <v>2867870</v>
+      </c>
+      <c r="K15" s="14">
+        <v>2236179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2012</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>3</v>
+      </c>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="4">
+        <v>2019</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2013</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3</v>
+      </c>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="C19" s="4">
+        <v>2015</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="C20" s="4">
+        <v>2016</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="C21" s="4">
+        <v>2017</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>4</v>
+      </c>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="C22" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>4</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="C23" s="4">
+        <v>2019</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>4</v>
+      </c>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="4">
+        <v>2020</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>4</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="4">
+        <v>2021</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>4</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="4">
+        <v>2022</v>
+      </c>
+      <c r="D26" s="4">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="M1" r:id="rId1" xr:uid="{8C8E38F7-3208-4ACA-A8B1-2CD5D828B29D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>